<commit_message>
changed first gardener dialog
</commit_message>
<xml_diff>
--- a/doc/dialog sources/�������� ������.xlsx
+++ b/doc/dialog sources/�������� ������.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="19920" windowHeight="7755"/>
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
-    <t>Существо появляется на экране. Надо сказать, оно не выглядит таким уж внеземным, скорее уж это нечто похоже на персонажа детского мультфильма. Оно смотрит на тебя… или возможно что смотрит, из черного  провала под шляпой. Ты даешь команду на включение прибора, оставленного капитаном Авроры, и пытаешься заговорить</t>
-  </si>
-  <si>
     <t>Вы... вы меня понимаете?</t>
   </si>
   <si>
@@ -166,16 +163,156 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
+    <t>Почему?</t>
+  </si>
+  <si>
+    <t>А… где она!? Где Аврора сейчас?! Вы знаете, вы можете ответить на этот вопрос?!</t>
+  </si>
+  <si>
+    <t>Потому что Аврора идет по своему пути. Вы – идете по своему.</t>
+  </si>
+  <si>
+    <t>Если вы расскажете мне где Аврора!! Где она?!! Я… я прошу вас! На нашей родной планете… нужен, необходим этот корабль! Он выполнял важную миссию!! Вся наша планета… буквально зависит от Авроры!!</t>
+  </si>
+  <si>
+    <t>Мы не можем рассказать вам. Вы следуете по своему пути, и вполне возможно, что вы встретите Аврору.</t>
+  </si>
+  <si>
+    <t>Ну уж нет, образина. Не знаю что, или как, но ты мне расскажешь. Иначе, клянусь, я разнесу тебя на куски!!</t>
+  </si>
+  <si>
+    <t>Хорошо. Свой путь. Мне кажется, вы употребляете это выражение не просто так. Что это означает?</t>
+  </si>
+  <si>
+    <t>Я соглашусь с вами, и проследую своим путем. Вполне возможно, что вы правы. Но я не понимаю вас. Что это значит?</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ни малейшей нотки злости в голосе</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Вы… необычны. Экипаж того, прошлого, тоже был необычным. Они тоже начали нам угрожать, но потом оказались способны нас понять.</t>
+    </r>
+  </si>
+  <si>
+    <t>А я буду не способен!! Ты по-прежнему отказываешься выдать мне координаты Авроры?!</t>
+  </si>
+  <si>
+    <t>Но поймите, множество людей умрут без данных имеющихся у Авроры, от нее очень многое зависит! Вы понимаете, как благодарна вам будет наша планета?!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В таком случае пеняй на себя!! </t>
+  </si>
+  <si>
+    <t>Да. Вы правы.</t>
+  </si>
+  <si>
+    <t>Не заступайте на чужой путь. Кроме того, ваша планета ничего не способна нам дать. Мы узнали это еще от Авроры.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я пытался!! Кто бы вы ни были, я вынужден вас атаковать!! Обстоятельства выше меня! </t>
+  </si>
+  <si>
+    <t>Мне тяжело это признавать, но хорошо! Хорошо! Что за путь, о чем вы говорите?!</t>
+  </si>
+  <si>
+    <r>
+      <t>Путь. Мы считаем, что каждое существо идет по своему пути. Тот, кто видит пути других и свои пути, не должен вольно или невольно пересекать их. Мы – видим. Мы – не пересекаем.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Вы…. Кто такие «Вы»? Что за «Вы»? Кто вы такие?</t>
+  </si>
+  <si>
+    <t>Я не понял. Что вы хотите мне сказать? Что мне сделать, чтобы найти Аврору?!</t>
+  </si>
+  <si>
+    <t>Видим…. Пересекаем…. Вы хотите сказать, что можете видеть будущее?</t>
+  </si>
+  <si>
+    <t>Мы – Садовники. Самое близкое значение, заключается именно в этом слове. Все вокруг – сад. Он не наш, мы просто можем выращивать растения, и видеть, как они растут. Мы не можем объяснить этого на вашем языке по иному, нам жаль.</t>
+  </si>
+  <si>
+    <t>Мы уже говорили – следовать своему пути. Умный и сильный найдет дорогу… или проложит ее.</t>
+  </si>
+  <si>
+    <t>Это не так. Мы не можем рассказать это полностью, вы просто не поймете этих ощущений. Мы разные. Просто поверьте, одно растение не может стать другим. Точно так же легко можно увидеть кто кем станет. Бывают исключения, но они очень редки.</t>
+  </si>
+  <si>
+    <t>Мне мало что понятно. Вы хотите чтобы мы следовали своим путем? Хорошо. Отлично. Вы правы. Но что это значит?</t>
+  </si>
+  <si>
+    <t>Ничего. У вас есть свой путь. Вы должны ему следовать. Мы не можем пересечь вашу дорогу, с дорогой Авроры, но можем поведать нечто иное.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Значит, следовать, говорите?! Хорошо, черт возьми. Тем лучше. Конец связи. </t>
+  </si>
+  <si>
+    <t>Хорошо.  Что вы хотите мне рассказать?</t>
+  </si>
+  <si>
+    <t>Мы знаем, что ваш народ уже вырос из своей колыбели, именно поэтому вы и находитесь здесь. Мы будем рады предоставить вам помощь. В меру своих сил, конечно.</t>
+  </si>
+  <si>
+    <t>А откуда… а, да. Аврора…. Хорошо. Приятно такое участие со стороны внеземной цивилизации. Вы хотите нам помочь?</t>
+  </si>
+  <si>
+    <t>Мы можем. Если ваша планета бедна ресурсами, вам стоит добывать их. Не бойтесь исчерпания – Вселенная бесконечна, и с каждой секундой она становится все бесконечнее, места в ней хватит всем.</t>
+  </si>
+  <si>
+    <t>Это просто замечательно. А что касается других… таких как вы? Существуют ли еще инопланетяне во Вселенной?</t>
+  </si>
+  <si>
+    <t>Конечно. Неужели вы не грезили о городах за небесами?</t>
+  </si>
+  <si>
+    <t>Как с ними связаться? Мы хотим заявить о себе.</t>
+  </si>
+  <si>
+    <r>
+      <t>А стоит ли….</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -185,36 +322,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Что?! Аврора?!! Вы видели Аврору?!!</t>
-    </r>
-  </si>
-  <si>
-    <t>Почему?</t>
-  </si>
-  <si>
-    <t>А… где она!? Где Аврора сейчас?! Вы знаете, вы можете ответить на этот вопрос?!</t>
-  </si>
-  <si>
-    <t>Потому что Аврора идет по своему пути. Вы – идете по своему.</t>
-  </si>
-  <si>
-    <t>Если вы расскажете мне где Аврора!! Где она?!! Я… я прошу вас! На нашей родной планете… нужен, необходим этот корабль! Он выполнял важную миссию!! Вся наша планета… буквально зависит от Авроры!!</t>
-  </si>
-  <si>
-    <t>Мы не можем рассказать вам. Вы следуете по своему пути, и вполне возможно, что вы встретите Аврору.</t>
-  </si>
-  <si>
-    <t>Ну уж нет, образина. Не знаю что, или как, но ты мне расскажешь. Иначе, клянусь, я разнесу тебя на куски!!</t>
-  </si>
-  <si>
-    <t>Хорошо. Свой путь. Мне кажется, вы употребляете это выражение не просто так. Что это означает?</t>
-  </si>
-  <si>
-    <t>Я соглашусь с вами, и проследую своим путем. Вполне возможно, что вы правы. Но я не понимаю вас. Что это значит?</t>
-  </si>
-  <si>
-    <r>
-      <t>*</t>
+      <t xml:space="preserve"> *</t>
     </r>
     <r>
       <rPr>
@@ -225,7 +333,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ни малейшей нотки злости в голосе</t>
+      <t>Садовник</t>
     </r>
     <r>
       <rPr>
@@ -236,6 +344,28 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>задумался. Это длится долго, но не более двух минут</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">* </t>
     </r>
     <r>
@@ -247,162 +377,6 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Вы… необычны. Экипаж того, прошлого, тоже был необычным. Они тоже начали нам угрожать, но потом оказались способны нас понять.</t>
-    </r>
-  </si>
-  <si>
-    <t>А я буду не способен!! Ты по-прежнему отказываешься выдать мне координаты Авроры?!</t>
-  </si>
-  <si>
-    <t>Но поймите, множество людей умрут без данных имеющихся у Авроры, от нее очень многое зависит! Вы понимаете, как благодарна вам будет наша планета?!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В таком случае пеняй на себя!! </t>
-  </si>
-  <si>
-    <t>Да. Вы правы.</t>
-  </si>
-  <si>
-    <t>Не заступайте на чужой путь. Кроме того, ваша планета ничего не способна нам дать. Мы узнали это еще от Авроры.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Я пытался!! Кто бы вы ни были, я вынужден вас атаковать!! Обстоятельства выше меня! </t>
-  </si>
-  <si>
-    <t>Мне тяжело это признавать, но хорошо! Хорошо! Что за путь, о чем вы говорите?!</t>
-  </si>
-  <si>
-    <r>
-      <t>Путь. Мы считаем, что каждое существо идет по своему пути. Тот, кто видит пути других и свои пути, не должен вольно или невольно пересекать их. Мы – видим. Мы – не пересекаем.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>Вы…. Кто такие «Вы»? Что за «Вы»? Кто вы такие?</t>
-  </si>
-  <si>
-    <t>Я не понял. Что вы хотите мне сказать? Что мне сделать, чтобы найти Аврору?!</t>
-  </si>
-  <si>
-    <t>Видим…. Пересекаем…. Вы хотите сказать, что можете видеть будущее?</t>
-  </si>
-  <si>
-    <t>Мы – Садовники. Самое близкое значение, заключается именно в этом слове. Все вокруг – сад. Он не наш, мы просто можем выращивать растения, и видеть, как они растут. Мы не можем объяснить этого на вашем языке по иному, нам жаль.</t>
-  </si>
-  <si>
-    <t>Мы уже говорили – следовать своему пути. Умный и сильный найдет дорогу… или проложит ее.</t>
-  </si>
-  <si>
-    <t>Это не так. Мы не можем рассказать это полностью, вы просто не поймете этих ощущений. Мы разные. Просто поверьте, одно растение не может стать другим. Точно так же легко можно увидеть кто кем станет. Бывают исключения, но они очень редки.</t>
-  </si>
-  <si>
-    <t>Мне мало что понятно. Вы хотите чтобы мы следовали своим путем? Хорошо. Отлично. Вы правы. Но что это значит?</t>
-  </si>
-  <si>
-    <t>Ничего. У вас есть свой путь. Вы должны ему следовать. Мы не можем пересечь вашу дорогу, с дорогой Авроры, но можем поведать нечто иное.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Значит, следовать, говорите?! Хорошо, черт возьми. Тем лучше. Конец связи. </t>
-  </si>
-  <si>
-    <t>Хорошо.  Что вы хотите мне рассказать?</t>
-  </si>
-  <si>
-    <t>Мы знаем, что ваш народ уже вырос из своей колыбели, именно поэтому вы и находитесь здесь. Мы будем рады предоставить вам помощь. В меру своих сил, конечно.</t>
-  </si>
-  <si>
-    <t>А откуда… а, да. Аврора…. Хорошо. Приятно такое участие со стороны внеземной цивилизации. Вы хотите нам помочь?</t>
-  </si>
-  <si>
-    <t>Мы можем. Если ваша планета бедна ресурсами, вам стоит добывать их. Не бойтесь исчерпания – Вселенная бесконечна, и с каждой секундой она становится все бесконечнее, места в ней хватит всем.</t>
-  </si>
-  <si>
-    <t>Это просто замечательно. А что касается других… таких как вы? Существуют ли еще инопланетяне во Вселенной?</t>
-  </si>
-  <si>
-    <t>Конечно. Неужели вы не грезили о городах за небесами?</t>
-  </si>
-  <si>
-    <t>Как с ними связаться? Мы хотим заявить о себе.</t>
-  </si>
-  <si>
-    <r>
-      <t>А стоит ли….</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> *</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Садовник</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>задумался. Это длится долго, но не более двух минут</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">* </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Пожалуй. С другой стороны планеты, находится космическая станция. Эти существа специализируются на общении и торговле. Они будут рады вам помочь.</t>
     </r>
   </si>
@@ -420,13 +394,19 @@
   </si>
   <si>
     <t>Вы все еще мне очень непонятны. Но, думаю да, наш диалог нельзя назвать бесполезным. Конец связи.</t>
+  </si>
+  <si>
+    <t>Что?! Аврора?!! Вы видели Аврору?!!</t>
+  </si>
+  <si>
+    <t>*существо появляется на экране. Оно похоже на описание, оставленное капитаном Авроры. Действительно, выглядит слишком уж… по-человечески. Глаза посверкивающие из под темного провала шляпы. Серый плащ, скрывающий тело. Его можно принять за человека. И оно ждет, пока ты что-то скажешь*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,20 +422,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -487,11 +453,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
+      <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,7 +548,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -617,7 +582,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -793,439 +757,439 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="68.5703125" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2">
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="B23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2">
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="B24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>26</v>
+    <row r="27" spans="1:3">
+      <c r="B27" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C27" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>27</v>
+    <row r="28" spans="1:3">
+      <c r="B28" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C28" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C30" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>27</v>
+    <row r="31" spans="1:3">
+      <c r="B31" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C31" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="2">
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>27</v>
+    <row r="34" spans="1:3">
+      <c r="B34" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C34" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="2">
         <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C37" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>26</v>
+    <row r="38" spans="1:3">
+      <c r="B38" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C38" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="2">
         <v>9</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="B40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C40" s="2">
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="B41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C41" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="2">
         <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C43" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="2">
         <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C45" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="2">
         <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C47" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="2">
         <v>18</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="B49" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C49" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="2">
         <v>20</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="B51" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C51" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="2">
         <v>21</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="B53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53" s="2">
         <v>-1</v>
@@ -1238,24 +1202,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>